<commit_message>
refactoring for router to templates.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bukun\AppData\Local\Temp\Mxt91\RemoteFiles\264404_3_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bukun\AppData\Local\Temp\Mxt91\RemoteFiles\67310_3_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -495,9 +495,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ta1</t>
-  </si>
-  <si>
     <t>t01</t>
   </si>
   <si>
@@ -513,31 +510,7 @@
     <t>t05</t>
   </si>
   <si>
-    <t>ta2</t>
-  </si>
-  <si>
     <t>t06</t>
-  </si>
-  <si>
-    <t>ta3</t>
-  </si>
-  <si>
-    <t>ta4</t>
-  </si>
-  <si>
-    <t>ta5</t>
-  </si>
-  <si>
-    <t>ta6</t>
-  </si>
-  <si>
-    <t>ta7</t>
-  </si>
-  <si>
-    <t>ta8</t>
-  </si>
-  <si>
-    <t>ta9</t>
   </si>
   <si>
     <t>Physical Geography</t>
@@ -545,6 +518,42 @@
   </si>
   <si>
     <t>agri</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t81</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t84</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t86</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t89</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1100,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2243,7 +2252,7 @@
     </row>
     <row r="3" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
@@ -3302,7 +3311,7 @@
     <row r="4" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>32</v>
@@ -3353,7 +3362,7 @@
     <row r="5" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>33</v>
@@ -3404,7 +3413,7 @@
     <row r="6" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>34</v>
@@ -3455,7 +3464,7 @@
     <row r="7" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>35</v>
@@ -3506,7 +3515,7 @@
     <row r="8" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>36</v>
@@ -3556,11 +3565,11 @@
     </row>
     <row r="9" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>123</v>
@@ -4613,7 +4622,7 @@
     <row r="10" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -4664,7 +4673,7 @@
     <row r="11" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>38</v>
@@ -4715,7 +4724,7 @@
     <row r="12" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>39</v>
@@ -4766,7 +4775,7 @@
     <row r="13" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>40</v>
@@ -4817,7 +4826,7 @@
     <row r="14" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>41</v>
@@ -4868,7 +4877,7 @@
     <row r="15" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>42</v>
@@ -4918,7 +4927,7 @@
     </row>
     <row r="16" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -5975,7 +5984,7 @@
     <row r="17" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>56</v>
@@ -6026,7 +6035,7 @@
     <row r="18" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>57</v>
@@ -6077,7 +6086,7 @@
     <row r="19" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>58</v>
@@ -6128,7 +6137,7 @@
     <row r="20" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>59</v>
@@ -6179,7 +6188,7 @@
     <row r="21" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>60</v>
@@ -6229,7 +6238,7 @@
     </row>
     <row r="22" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>119</v>
@@ -7281,7 +7290,7 @@
     <row r="23" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>66</v>
@@ -7330,7 +7339,7 @@
     <row r="24" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>67</v>
@@ -7377,7 +7386,7 @@
     <row r="25" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>68</v>
@@ -7423,7 +7432,7 @@
     </row>
     <row r="26" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -8484,7 +8493,7 @@
     <row r="27" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>72</v>
@@ -8541,7 +8550,7 @@
     <row r="28" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>73</v>
@@ -8596,7 +8605,7 @@
     <row r="29" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>74</v>
@@ -8651,7 +8660,7 @@
     <row r="30" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>75</v>
@@ -8705,7 +8714,7 @@
     </row>
     <row r="31" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
@@ -9768,7 +9777,7 @@
     <row r="32" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>80</v>
@@ -9827,7 +9836,7 @@
     <row r="33" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>81</v>
@@ -9885,7 +9894,7 @@
     </row>
     <row r="34" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>114</v>
@@ -10947,7 +10956,7 @@
     <row r="35" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>82</v>
@@ -11006,7 +11015,7 @@
     <row r="36" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>83</v>
@@ -11063,7 +11072,7 @@
     <row r="37" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>84</v>
@@ -11122,7 +11131,7 @@
     <row r="38" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>85</v>
@@ -11181,7 +11190,7 @@
     <row r="39" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>86</v>
@@ -11239,7 +11248,7 @@
     </row>
     <row r="40" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>111</v>
@@ -12293,7 +12302,7 @@
     <row r="41" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>87</v>
@@ -12344,7 +12353,7 @@
     <row r="42" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>88</v>
@@ -12395,7 +12404,7 @@
     <row r="43" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>89</v>
@@ -12446,7 +12455,7 @@
     <row r="44" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>90</v>
@@ -12496,11 +12505,11 @@
     </row>
     <row r="45" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>110</v>
@@ -13551,7 +13560,7 @@
     <row r="46" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>91</v>
@@ -13600,7 +13609,7 @@
     <row r="47" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>92</v>
@@ -13649,7 +13658,7 @@
     <row r="48" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>93</v>
@@ -13698,7 +13707,7 @@
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Move the `slug` to the beginning of the cell in XLXS file.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bukun\AppData\Local\Temp\Mxt91\RemoteFiles\67310_3_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opt\github\TorCMS\database\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,58 +14,13 @@
   <sheets>
     <sheet name="geodata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
   <si>
-    <t>Record,record</t>
-  </si>
-  <si>
-    <t>Derive,derive</t>
-  </si>
-  <si>
-    <t>Temperal,temperal</t>
-  </si>
-  <si>
-    <t>Spatial,spatial</t>
-  </si>
-  <si>
-    <t>Resolution,resolution</t>
-  </si>
-  <si>
-    <t>Share_type,share_type</t>
-  </si>
-  <si>
-    <t>Storage,storage</t>
-  </si>
-  <si>
-    <t>View_class,view_class</t>
-  </si>
-  <si>
-    <t>Degree,degree</t>
-  </si>
-  <si>
-    <t>Paper_type,paper_type</t>
-  </si>
-  <si>
-    <t>Vectype,vectype</t>
-  </si>
-  <si>
-    <t>Rastype,rastype</t>
-  </si>
-  <si>
-    <t>Media_type,media_type</t>
-  </si>
-  <si>
-    <t>Filetype,filetype</t>
-  </si>
-  <si>
-    <t>Size,size</t>
-  </si>
-  <si>
     <t>RS Image,GIS Data,Document,Multimedia,Formatted Data</t>
   </si>
   <si>
@@ -185,12 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Grade,grade</t>
-  </si>
-  <si>
-    <t>Serial,serial</t>
-  </si>
-  <si>
     <t>重力</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -555,6 +504,57 @@
   <si>
     <t>t89</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>record,Record</t>
+  </si>
+  <si>
+    <t>derive,Derive</t>
+  </si>
+  <si>
+    <t>grade,Grade</t>
+  </si>
+  <si>
+    <t>serial,Serial</t>
+  </si>
+  <si>
+    <t>temperal,Temperal</t>
+  </si>
+  <si>
+    <t>spatial,Spatial</t>
+  </si>
+  <si>
+    <t>resolution,Resolution</t>
+  </si>
+  <si>
+    <t>share_type,Share_type</t>
+  </si>
+  <si>
+    <t>storage,Storage</t>
+  </si>
+  <si>
+    <t>view_class,View_class</t>
+  </si>
+  <si>
+    <t>degree,Degree</t>
+  </si>
+  <si>
+    <t>paper_type,Paper_type</t>
+  </si>
+  <si>
+    <t>vectype,Vectype</t>
+  </si>
+  <si>
+    <t>rastype,Rastype</t>
+  </si>
+  <si>
+    <t>media_type,Media_type</t>
+  </si>
+  <si>
+    <t>filetype,Filetype</t>
+  </si>
+  <si>
+    <t>size,Size</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:AML49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1119,7 +1119,8 @@
     <col min="2" max="2" width="13.44140625" style="4"/>
     <col min="3" max="3" width="25" style="4"/>
     <col min="4" max="4" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.21875" style="4"/>
+    <col min="5" max="5" width="30.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.21875" style="4"/>
     <col min="9" max="9" width="12.5546875" style="4"/>
     <col min="10" max="1026" width="9.21875" style="4"/>
     <col min="1027" max="16384" width="8.88671875" style="2"/>
@@ -1131,61 +1132,61 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>8</v>
+        <v>138</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -2199,67 +2200,67 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="U2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -3311,13 +3312,13 @@
     <row r="4" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
@@ -3362,13 +3363,13 @@
     <row r="5" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
@@ -3413,13 +3414,13 @@
     <row r="6" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -3464,13 +3465,13 @@
     <row r="7" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -3515,13 +3516,13 @@
     <row r="8" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
@@ -3565,14 +3566,14 @@
     </row>
     <row r="9" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -4622,13 +4623,13 @@
     <row r="10" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E10" s="10">
         <v>1</v>
@@ -4673,13 +4674,13 @@
     <row r="11" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -4724,13 +4725,13 @@
     <row r="12" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10">
         <v>1</v>
@@ -4775,13 +4776,13 @@
     <row r="13" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -4826,13 +4827,13 @@
     <row r="14" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
@@ -4877,13 +4878,13 @@
     <row r="15" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -4927,14 +4928,14 @@
     </row>
     <row r="16" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
@@ -5984,13 +5985,13 @@
     <row r="17" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -6035,13 +6036,13 @@
     <row r="18" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>
@@ -6086,13 +6087,13 @@
     <row r="19" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
@@ -6137,13 +6138,13 @@
     <row r="20" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E20" s="10">
         <v>1</v>
@@ -6188,13 +6189,13 @@
     <row r="21" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E21" s="10">
         <v>1</v>
@@ -6238,13 +6239,13 @@
     </row>
     <row r="22" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E22" s="6">
         <v>1</v>
@@ -7290,13 +7291,13 @@
     <row r="23" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E23" s="10">
         <v>1</v>
@@ -7339,13 +7340,13 @@
     <row r="24" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E24" s="10">
         <v>1</v>
@@ -7386,13 +7387,13 @@
     <row r="25" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E25" s="10">
         <v>1</v>
@@ -7432,14 +7433,14 @@
     </row>
     <row r="26" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
@@ -8493,13 +8494,13 @@
     <row r="27" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -8550,13 +8551,13 @@
     <row r="28" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E28" s="10">
         <v>1</v>
@@ -8605,13 +8606,13 @@
     <row r="29" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E29" s="10">
         <v>1</v>
@@ -8660,13 +8661,13 @@
     <row r="30" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E30" s="10">
         <v>1</v>
@@ -8714,14 +8715,14 @@
     </row>
     <row r="31" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="E31" s="6">
         <v>1</v>
@@ -9777,13 +9778,13 @@
     <row r="32" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E32" s="10">
         <v>1</v>
@@ -9836,13 +9837,13 @@
     <row r="33" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E33" s="10">
         <v>1</v>
@@ -9894,13 +9895,13 @@
     </row>
     <row r="34" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
@@ -10956,13 +10957,13 @@
     <row r="35" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E35" s="10">
         <v>1</v>
@@ -11015,13 +11016,13 @@
     <row r="36" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E36" s="10">
         <v>1</v>
@@ -11072,13 +11073,13 @@
     <row r="37" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E37" s="10">
         <v>1</v>
@@ -11131,13 +11132,13 @@
     <row r="38" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E38" s="10">
         <v>1</v>
@@ -11190,13 +11191,13 @@
     <row r="39" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="E39" s="10">
         <v>1</v>
@@ -11248,13 +11249,13 @@
     </row>
     <row r="40" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
@@ -12302,13 +12303,13 @@
     <row r="41" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E41" s="10">
         <v>1</v>
@@ -12353,13 +12354,13 @@
     <row r="42" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E42" s="10">
         <v>1</v>
@@ -12404,13 +12405,13 @@
     <row r="43" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E43" s="10">
         <v>1</v>
@@ -12455,13 +12456,13 @@
     <row r="44" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
@@ -12505,14 +12506,14 @@
     </row>
     <row r="45" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E45" s="6">
         <v>1</v>
@@ -13560,13 +13561,13 @@
     <row r="46" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E46" s="10">
         <v>1</v>
@@ -13609,13 +13610,13 @@
     <row r="47" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="9" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E47" s="10">
         <v>1</v>
@@ -13658,13 +13659,13 @@
     <row r="48" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E48" s="10">
         <v>1</v>
@@ -13707,13 +13708,13 @@
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E49" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
Add valication for CRUD.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="geodata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -69,9 +69,6 @@
     <t>Text,Pdf,Scansion</t>
   </si>
   <si>
-    <t>Mb</t>
-  </si>
-  <si>
     <t>marine physics</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -561,7 +558,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>-</t>
+    <t>email:Mb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1117,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="X47" sqref="X47"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1140,64 +1141,64 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -2258,7 +2259,7 @@
         <v>15</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>146</v>
@@ -2266,14 +2267,14 @@
     </row>
     <row r="3" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -3327,13 +3328,13 @@
     <row r="4" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
@@ -3381,13 +3382,13 @@
     <row r="5" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
@@ -3435,13 +3436,13 @@
     <row r="6" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -3489,13 +3490,13 @@
     <row r="7" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -3543,13 +3544,13 @@
     <row r="8" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
@@ -3596,14 +3597,14 @@
     </row>
     <row r="9" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -4655,13 +4656,13 @@
     <row r="10" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10">
         <v>1</v>
@@ -4709,13 +4710,13 @@
     <row r="11" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -4763,13 +4764,13 @@
     <row r="12" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="10">
         <v>1</v>
@@ -4817,13 +4818,13 @@
     <row r="13" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -4871,13 +4872,13 @@
     <row r="14" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
@@ -4925,13 +4926,13 @@
     <row r="15" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -4978,14 +4979,14 @@
     </row>
     <row r="16" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
@@ -6037,13 +6038,13 @@
     <row r="17" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -6091,13 +6092,13 @@
     <row r="18" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>
@@ -6145,13 +6146,13 @@
     <row r="19" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
@@ -6199,13 +6200,13 @@
     <row r="20" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="10">
         <v>1</v>
@@ -6253,13 +6254,13 @@
     <row r="21" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="10">
         <v>1</v>
@@ -6306,13 +6307,13 @@
     </row>
     <row r="22" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="E22" s="6">
         <v>1</v>
@@ -7360,13 +7361,13 @@
     <row r="23" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="10">
         <v>1</v>
@@ -7412,13 +7413,13 @@
     <row r="24" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="10">
         <v>1</v>
@@ -7462,13 +7463,13 @@
     <row r="25" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="10">
         <v>1</v>
@@ -7511,14 +7512,14 @@
     </row>
     <row r="26" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
@@ -8574,13 +8575,13 @@
     <row r="27" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -8634,13 +8635,13 @@
     <row r="28" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="10">
         <v>1</v>
@@ -8692,13 +8693,13 @@
     <row r="29" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="10">
         <v>1</v>
@@ -8750,13 +8751,13 @@
     <row r="30" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="10">
         <v>1</v>
@@ -8807,14 +8808,14 @@
     </row>
     <row r="31" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E31" s="6">
         <v>1</v>
@@ -9872,13 +9873,13 @@
     <row r="32" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="10">
         <v>1</v>
@@ -9934,13 +9935,13 @@
     <row r="33" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" s="10">
         <v>1</v>
@@ -9995,13 +9996,13 @@
     </row>
     <row r="34" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
@@ -11059,13 +11060,13 @@
     <row r="35" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="10">
         <v>1</v>
@@ -11121,13 +11122,13 @@
     <row r="36" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E36" s="10">
         <v>1</v>
@@ -11181,13 +11182,13 @@
     <row r="37" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="10">
         <v>1</v>
@@ -11243,13 +11244,13 @@
     <row r="38" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E38" s="10">
         <v>1</v>
@@ -11305,13 +11306,13 @@
     <row r="39" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="10">
         <v>1</v>
@@ -11366,13 +11367,13 @@
     </row>
     <row r="40" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
@@ -12422,13 +12423,13 @@
     <row r="41" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41" s="10">
         <v>1</v>
@@ -12476,13 +12477,13 @@
     <row r="42" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" s="10">
         <v>1</v>
@@ -12530,13 +12531,13 @@
     <row r="43" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E43" s="10">
         <v>1</v>
@@ -12584,13 +12585,13 @@
     <row r="44" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
@@ -12637,14 +12638,14 @@
     </row>
     <row r="45" spans="1:1026" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45" s="6">
         <v>1</v>
@@ -13694,13 +13695,13 @@
     <row r="46" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" s="10">
         <v>1</v>
@@ -13746,13 +13747,13 @@
     <row r="47" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="10">
         <v>1</v>
@@ -13798,13 +13799,13 @@
     <row r="48" spans="1:1026" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E48" s="10">
         <v>1</v>
@@ -13850,13 +13851,13 @@
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E49" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
fix for entity downloading.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -570,15 +570,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>memo,Memo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>contact_email,Contact Email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>texx</t>
+    <t>file_download,Download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>download</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:AML49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1217,10 +1217,10 @@
         <v>144</v>
       </c>
       <c r="W1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>

</xml_diff>

<commit_message>
fix bugs. Update default HTML.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-post" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="2-data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="9-data" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="m-map" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -319,6 +319,7 @@
       <color rgb="FF080808"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -513,7 +514,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="1" sqref="B16:B17 D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -644,8 +645,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -662,7 +663,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -809,8 +810,8 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="1" sqref="B16:B17 D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,10 +1062,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B16:B17 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add module for widghet menu.
</commit_message>
<xml_diff>
--- a/database/meta/info_tags.xlsx
+++ b/database/meta/info_tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opt\github\TorCMS\database\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED8DBE-1BBB-4431-A025-A65273329A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A130D7-3615-4380-8695-13F050E0FAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,36 +91,15 @@
     <t>Economic resources</t>
   </si>
   <si>
-    <t>eco_res</t>
-  </si>
-  <si>
     <t>Nature resources</t>
   </si>
   <si>
-    <t>nature_res</t>
-  </si>
-  <si>
-    <t>nature_resources</t>
-  </si>
-  <si>
-    <t>t22</t>
-  </si>
-  <si>
     <t>Nature Geographic</t>
   </si>
   <si>
-    <t>nature_geo</t>
-  </si>
-  <si>
     <t>Basic geographic</t>
   </si>
   <si>
-    <t>basic_geo_db</t>
-  </si>
-  <si>
-    <t>t21</t>
-  </si>
-  <si>
     <t>Raw,Rough,Finish,Product</t>
   </si>
   <si>
@@ -137,6 +116,34 @@
   </si>
   <si>
     <t>_record,Record</t>
+  </si>
+  <si>
+    <t>t31</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>t32</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic_geo_db3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>nature_geo3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>nature_resources3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>nature_res3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>eco_res3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -795,7 +802,7 @@
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="17.25"/>
@@ -822,13 +829,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="71.25">
@@ -837,13 +844,13 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -852,10 +859,10 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
@@ -871,10 +878,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -886,14 +893,14 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
@@ -909,10 +916,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
@@ -928,7 +935,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>

</xml_diff>